<commit_message>
added overview and MECH-shooter text
@chrishu001
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zzhih\Desktop\ME210_Team24_Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E7F16D-9CE4-4481-8953-563FA3B12379}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8214B8-80F0-4A9D-BBDD-63ED5357643E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>M5 Washer</t>
-  </si>
-  <si>
-    <t>Servor Motor</t>
   </si>
   <si>
     <t>Chassis</t>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>1/8" half coupler</t>
+  </si>
+  <si>
+    <t>Servo Motor</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -615,10 +615,10 @@
     <row r="1" spans="1:27" s="7" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>0</v>
@@ -736,7 +736,7 @@
     <row r="4" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -776,7 +776,7 @@
     <row r="5" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -1056,7 +1056,7 @@
     <row r="12" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -1095,10 +1095,10 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="2">
         <v>4</v>
@@ -1138,7 +1138,7 @@
     <row r="14" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2">
         <v>4</v>
@@ -1147,7 +1147,7 @@
         <v>6.88</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
@@ -1178,7 +1178,7 @@
     <row r="15" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
@@ -1218,7 +1218,7 @@
     <row r="16" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2">
         <v>4</v>
@@ -1258,7 +1258,7 @@
     <row r="17" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2">
         <v>1</v>
@@ -1298,7 +1298,7 @@
     <row r="18" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2">
         <v>4</v>
@@ -1338,7 +1338,7 @@
     <row r="19" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2">
         <v>12</v>
@@ -1377,10 +1377,10 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
@@ -1420,7 +1420,7 @@
     <row r="21" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
@@ -1429,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="0"/>
@@ -1460,7 +1460,7 @@
     <row r="22" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="B22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
@@ -1469,7 +1469,7 @@
         <v>14.95</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="0"/>
@@ -1500,7 +1500,7 @@
     <row r="23" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="B23" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="2">
         <v>1</v>
@@ -1509,7 +1509,7 @@
         <v>14.95</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="0"/>
@@ -1539,10 +1539,10 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="2">
         <v>2</v>
@@ -1582,7 +1582,7 @@
     <row r="25" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="2">
         <v>2</v>
@@ -1654,7 +1654,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27" s="3">
         <f>SUM(F2:F25)</f>

</xml_diff>